<commit_message>
update code regularly, 30 Aug
</commit_message>
<xml_diff>
--- a/experiments/NN_hyperparameter-tuning/ntu_rgb_d_tuning_history_data/ntu_rgb_d_NN_RandomSearch-tuning.xlsx
+++ b/experiments/NN_hyperparameter-tuning/ntu_rgb_d_tuning_history_data/ntu_rgb_d_NN_RandomSearch-tuning.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\poland\PW\Thesis\Projects\humiact-proj\experiments\NN_hyperparameter-tuning\ntu_rgb_d_tuning_history_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C8941-C10D-4578-BCF7-5380CFF87615}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C4C7C-A6C4-4A92-B361-FD3C97035F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomSearch_Tuner" sheetId="1" r:id="rId1"/>
     <sheet name="Models-based-on-my_smallsearch" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparison" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
   <si>
     <t>layers:</t>
   </si>
@@ -92,6 +93,24 @@
   </si>
   <si>
     <t>cs,skips=2</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>NN-GridSearch</t>
+  </si>
+  <si>
+    <t>NN-RandomSearch</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -168,12 +187,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -184,8 +197,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -217,11 +236,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -247,28 +279,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -296,8 +316,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -311,39 +352,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,6 +411,1143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$4:$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN-GridSearch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NN-RandomSearch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.75080000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88429999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85919999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-51C6-4065-804A-26A4FA077F56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$4:$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN-GridSearch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NN-RandomSearch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$E$4:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.69169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-51C6-4065-804A-26A4FA077F56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Comparison!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Comparison!$C$4:$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN-GridSearch</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NN-RandomSearch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Comparison!$F$4:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.4425</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45040000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-51C6-4065-804A-26A4FA077F56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:axId val="1850799167"/>
+        <c:axId val="1850797087"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1850799167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850797087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1850797087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1850799167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="225">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1286,6 +2475,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F229928-CE88-4F6B-A00D-51314DFDE3CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1551,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J12"/>
+    <sheetView topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,249 +2801,229 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="36">
         <v>1</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34">
+      <c r="D3" s="36"/>
+      <c r="E3" s="37">
         <v>2</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34">
+      <c r="F3" s="37"/>
+      <c r="G3" s="37">
         <v>3</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34">
+      <c r="H3" s="37"/>
+      <c r="I3" s="38">
         <v>4</v>
       </c>
-      <c r="J3" s="34"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="2:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="28">
         <v>3</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="28">
         <v>2</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>600</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="28">
         <v>200</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="28">
         <v>400</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="36">
+      <c r="J5" s="40">
         <v>600</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="32"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="40" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="32"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="13">
+        <v>4.9465752773930496E-4</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="13">
-        <v>700</v>
-      </c>
-      <c r="E7" s="35" t="s">
+      <c r="F7" s="28">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="36">
-        <v>1000</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="38">
+      <c r="H7" s="30">
         <v>600</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="44">
+      <c r="J7" s="41">
         <v>1.4221828280940401E-3</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="32"/>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.17068649828433899</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="F8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="G8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="H8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="45">
+      <c r="J8" s="43">
         <v>0.17290469507376299</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13">
-        <v>900</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="36">
+      <c r="F9" s="28">
         <v>200</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="32">
         <v>5.3362330939185295E-4</v>
       </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="40"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="32"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="F10" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="33">
         <v>0.180631925662358</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="32"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="35"/>
+      <c r="E11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="16">
-        <v>4.9465752773930496E-4</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="44">
+      <c r="F11" s="32">
         <v>1.4763284782764601E-4</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="32"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="35"/>
+      <c r="E12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="18">
-        <v>0.17068649828433899</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="44">
+      <c r="F12" s="32">
         <v>0.15603390832742001</v>
       </c>
     </row>
@@ -1825,40 +3035,40 @@
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>600</v>
       </c>
       <c r="D17"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="13">
         <v>4.9465752773930496E-4</v>
       </c>
     </row>
@@ -1874,7 +3084,7 @@
       <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="15">
         <v>0.85919999999999996</v>
       </c>
     </row>
@@ -1882,7 +3092,7 @@
       <c r="B24" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="15">
         <v>0.748</v>
       </c>
     </row>
@@ -1890,7 +3100,7 @@
       <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="15">
         <v>0.45040000000000002</v>
       </c>
     </row>
@@ -1903,100 +3113,100 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="20"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="20"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="16"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="20"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="20"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="20"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="16"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="20"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="16"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="21"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="20"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="16"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="20"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="16"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="21"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="23"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="20"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="16"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="21"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="20"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="21"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="20"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="16"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="21"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="20"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="21"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="20"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="21"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="20"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="16"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="28"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="24"/>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" s="5" t="s">
@@ -2004,34 +3214,34 @@
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C109" s="15">
+      <c r="C109" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C110" s="15">
+      <c r="C110" s="12">
         <v>600</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C111" s="15" t="s">
+      <c r="C111" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C112" s="16">
+      <c r="C112" s="13">
         <v>1.4221828280940401E-3</v>
       </c>
     </row>
@@ -2067,7 +3277,7 @@
   <dimension ref="B4:C50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2079,39 +3289,39 @@
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="26">
         <v>700</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>1E-3</v>
       </c>
     </row>
@@ -2127,7 +3337,7 @@
       <c r="B12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="15">
         <v>0.88429999999999997</v>
       </c>
     </row>
@@ -2135,7 +3345,7 @@
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="15">
         <v>0.76629999999999998</v>
       </c>
     </row>
@@ -2143,7 +3353,7 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="15">
         <v>0.45179999999999998</v>
       </c>
     </row>
@@ -2151,39 +3361,39 @@
       <c r="B40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="26">
         <v>2000</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="13">
         <v>1E-3</v>
       </c>
     </row>
@@ -2199,7 +3409,7 @@
       <c r="B48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="15">
         <v>0.9698</v>
       </c>
     </row>
@@ -2207,7 +3417,7 @@
       <c r="B49" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="15">
         <v>0.84</v>
       </c>
     </row>
@@ -2215,7 +3425,7 @@
       <c r="B50" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="15">
         <v>0.44319999999999998</v>
       </c>
     </row>
@@ -2224,4 +3434,76 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FABCE9-08DF-4790-B5D4-A3E51CD9A6CD}">
+  <dimension ref="C3:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="52">
+        <v>0.75080000000000002</v>
+      </c>
+      <c r="E4" s="52">
+        <v>0.69169999999999998</v>
+      </c>
+      <c r="F4" s="52">
+        <v>0.4425</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="52">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="E5" s="52">
+        <v>0.76629999999999998</v>
+      </c>
+      <c r="F5" s="52">
+        <v>0.45179999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="52">
+        <v>0.85919999999999996</v>
+      </c>
+      <c r="E6" s="53">
+        <v>0.748</v>
+      </c>
+      <c r="F6" s="53">
+        <v>0.45040000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>